<commit_message>
FMX-1025: Support of auto-dispatching.
</commit_message>
<xml_diff>
--- a/apps/resources/categories_mapping_new.xlsx
+++ b/apps/resources/categories_mapping_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,18 +45,21 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -68,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="219">
   <si>
     <t xml:space="preserve">Anicennes catégories</t>
   </si>
@@ -112,7 +115,7 @@
     <t xml:space="preserve">NEW LVL 4 ID</t>
   </si>
   <si>
-    <t xml:space="preserve">ABPTYPE ID</t>
+    <t xml:space="preserve">ABP TYPE ID</t>
   </si>
   <si>
     <t xml:space="preserve">ABP NATURE ID</t>
@@ -602,6 +605,18 @@
   </si>
   <si>
     <t xml:space="preserve">Lvl 4 ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto-dispatching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABP Type ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABP Nature ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABP Bagtype ID</t>
   </si>
   <si>
     <t xml:space="preserve">Coating</t>
@@ -722,7 +737,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -760,12 +775,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -889,7 +898,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -926,10 +935,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -950,7 +955,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -962,11 +967,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1062,30 +1071,30 @@
   </sheetPr>
   <dimension ref="1:208"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S26" activeCellId="0" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.919028340081"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.3603238866397"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
@@ -1167,7 +1176,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>29</v>
       </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -1200,28 +1209,28 @@
       <c r="L3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="8" t="n">
         <f aca="false">E3+1000</f>
         <v>1002</v>
       </c>
-      <c r="N3" s="9" t="n">
+      <c r="N3" s="8" t="n">
         <v>2000</v>
       </c>
-      <c r="O3" s="9" t="n">
+      <c r="O3" s="8" t="n">
         <f aca="false">G3+3000</f>
         <v>3029</v>
       </c>
-      <c r="P3" s="10" t="n">
+      <c r="P3" s="9" t="n">
         <f aca="false">P173</f>
         <v>4001</v>
       </c>
-      <c r="Q3" s="10" t="n">
+      <c r="Q3" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="R3" s="10" t="n">
+      <c r="R3" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="S3" s="10" t="n">
+      <c r="S3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="AMF3" s="0"/>
@@ -1251,7 +1260,7 @@
         <v>30</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="8" t="str">
+      <c r="I4" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1262,14 +1271,14 @@
         <v>26</v>
       </c>
       <c r="L4" s="0"/>
-      <c r="M4" s="11" t="n">
+      <c r="M4" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N4" s="9" t="n">
+      <c r="N4" s="8" t="n">
         <v>2001</v>
       </c>
-      <c r="O4" s="9" t="n">
+      <c r="O4" s="8" t="n">
         <f aca="false">G4+3000</f>
         <v>3030</v>
       </c>
@@ -1302,7 +1311,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="8" t="str">
+      <c r="I5" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1313,22 +1322,22 @@
         <v>28</v>
       </c>
       <c r="L5" s="0"/>
-      <c r="M5" s="11" t="n">
+      <c r="M5" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N5" s="11" t="n">
+      <c r="N5" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O5" s="9" t="n">
+      <c r="O5" s="8" t="n">
         <f aca="false">G5+3000</f>
         <v>3031</v>
       </c>
       <c r="P5" s="0"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -1351,7 +1360,7 @@
         <v>32</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="8" t="str">
+      <c r="I6" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1364,18 +1373,18 @@
       <c r="L6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="11" t="n">
+      <c r="M6" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N6" s="9" t="n">
+      <c r="N6" s="8" t="n">
         <v>2002</v>
       </c>
-      <c r="O6" s="9" t="n">
+      <c r="O6" s="8" t="n">
         <f aca="false">G6+3000</f>
         <v>3032</v>
       </c>
-      <c r="P6" s="9" t="n">
+      <c r="P6" s="8" t="n">
         <v>4010</v>
       </c>
       <c r="Q6" s="0" t="n">
@@ -1406,7 +1415,7 @@
         <v>78</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="8" t="str">
+      <c r="I7" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1417,22 +1426,22 @@
         <v>34</v>
       </c>
       <c r="L7" s="0"/>
-      <c r="M7" s="11" t="n">
+      <c r="M7" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N7" s="11" t="n">
+      <c r="N7" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O7" s="11" t="n">
+      <c r="O7" s="10" t="n">
         <f aca="false">O5</f>
         <v>3031</v>
       </c>
       <c r="P7" s="0"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
@@ -1455,7 +1464,7 @@
         <v>79</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="8" t="str">
+      <c r="I8" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1468,15 +1477,15 @@
       <c r="L8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="11" t="n">
+      <c r="M8" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N8" s="11" t="n">
+      <c r="N8" s="10" t="n">
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O8" s="11" t="n">
+      <c r="O8" s="10" t="n">
         <f aca="false">O6</f>
         <v>3032</v>
       </c>
@@ -1512,7 +1521,7 @@
         <v>76</v>
       </c>
       <c r="H9" s="7"/>
-      <c r="I9" s="8" t="str">
+      <c r="I9" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1525,15 +1534,15 @@
       <c r="L9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="11" t="n">
+      <c r="M9" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N9" s="11" t="n">
+      <c r="N9" s="10" t="n">
         <f aca="false">N3</f>
         <v>2000</v>
       </c>
-      <c r="O9" s="11" t="n">
+      <c r="O9" s="10" t="n">
         <f aca="false">O3</f>
         <v>3029</v>
       </c>
@@ -1572,7 +1581,7 @@
         <v>77</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="8" t="str">
+      <c r="I10" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1583,15 +1592,15 @@
         <v>36</v>
       </c>
       <c r="L10" s="0"/>
-      <c r="M10" s="11" t="n">
+      <c r="M10" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N10" s="11" t="n">
+      <c r="N10" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O10" s="11" t="n">
+      <c r="O10" s="10" t="n">
         <f aca="false">O4</f>
         <v>3030</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>54</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="I11" s="8" t="str">
+      <c r="I11" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1637,15 +1646,15 @@
       <c r="L11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="11" t="n">
+      <c r="M11" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N11" s="11" t="n">
+      <c r="N11" s="10" t="n">
         <f aca="false">N3</f>
         <v>2000</v>
       </c>
-      <c r="O11" s="11" t="n">
+      <c r="O11" s="10" t="n">
         <f aca="false">O3</f>
         <v>3029</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>55</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="I12" s="8" t="str">
+      <c r="I12" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1695,15 +1704,15 @@
         <v>36</v>
       </c>
       <c r="L12" s="0"/>
-      <c r="M12" s="11" t="n">
+      <c r="M12" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N12" s="11" t="n">
+      <c r="N12" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O12" s="11" t="n">
+      <c r="O12" s="10" t="n">
         <f aca="false">O4</f>
         <v>3030</v>
       </c>
@@ -1736,7 +1745,7 @@
         <v>56</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="8" t="str">
+      <c r="I13" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1747,22 +1756,22 @@
         <v>27</v>
       </c>
       <c r="L13" s="0"/>
-      <c r="M13" s="11" t="n">
+      <c r="M13" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N13" s="11" t="n">
+      <c r="N13" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O13" s="11" t="n">
+      <c r="O13" s="10" t="n">
         <f aca="false">O5</f>
         <v>3031</v>
       </c>
       <c r="P13" s="0"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
@@ -1785,7 +1794,7 @@
         <v>57</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="8" t="str">
+      <c r="I14" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1798,15 +1807,15 @@
       <c r="L14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="11" t="n">
+      <c r="M14" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N14" s="11" t="n">
+      <c r="N14" s="10" t="n">
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O14" s="11" t="n">
+      <c r="O14" s="10" t="n">
         <f aca="false">O6</f>
         <v>3032</v>
       </c>
@@ -1842,7 +1851,7 @@
         <v>101</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="8" t="str">
+      <c r="I15" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1855,15 +1864,15 @@
       <c r="L15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M15" s="11" t="n">
+      <c r="M15" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N15" s="11" t="n">
+      <c r="N15" s="10" t="n">
         <f aca="false">N3</f>
         <v>2000</v>
       </c>
-      <c r="O15" s="11" t="n">
+      <c r="O15" s="10" t="n">
         <f aca="false">O3</f>
         <v>3029</v>
       </c>
@@ -1902,7 +1911,7 @@
         <v>102</v>
       </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="8" t="str">
+      <c r="I16" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1913,15 +1922,15 @@
         <v>36</v>
       </c>
       <c r="L16" s="0"/>
-      <c r="M16" s="11" t="n">
+      <c r="M16" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N16" s="11" t="n">
+      <c r="N16" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O16" s="11" t="n">
+      <c r="O16" s="10" t="n">
         <f aca="false">O4</f>
         <v>3030</v>
       </c>
@@ -1954,7 +1963,7 @@
         <v>103</v>
       </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="8" t="str">
+      <c r="I17" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -1965,22 +1974,22 @@
         <v>27</v>
       </c>
       <c r="L17" s="0"/>
-      <c r="M17" s="11" t="n">
+      <c r="M17" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N17" s="11" t="n">
+      <c r="N17" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O17" s="11" t="n">
+      <c r="O17" s="10" t="n">
         <f aca="false">O5</f>
         <v>3031</v>
       </c>
       <c r="P17" s="0"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
@@ -2003,7 +2012,7 @@
         <v>104</v>
       </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="8" t="str">
+      <c r="I18" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -2016,15 +2025,15 @@
       <c r="L18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="11" t="n">
+      <c r="M18" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N18" s="11" t="n">
+      <c r="N18" s="10" t="n">
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O18" s="11" t="n">
+      <c r="O18" s="10" t="n">
         <f aca="false">O6</f>
         <v>3032</v>
       </c>
@@ -2060,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="8" t="str">
+      <c r="I19" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -2073,15 +2082,15 @@
       <c r="L19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M19" s="11" t="n">
+      <c r="M19" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N19" s="11" t="n">
+      <c r="N19" s="10" t="n">
         <f aca="false">N3</f>
         <v>2000</v>
       </c>
-      <c r="O19" s="11" t="n">
+      <c r="O19" s="10" t="n">
         <f aca="false">O3</f>
         <v>3029</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="8" t="str">
+      <c r="I20" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -2131,15 +2140,15 @@
         <v>36</v>
       </c>
       <c r="L20" s="0"/>
-      <c r="M20" s="11" t="n">
+      <c r="M20" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N20" s="11" t="n">
+      <c r="N20" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O20" s="11" t="n">
+      <c r="O20" s="10" t="n">
         <f aca="false">O4</f>
         <v>3030</v>
       </c>
@@ -2172,7 +2181,7 @@
         <v>6</v>
       </c>
       <c r="H21" s="7"/>
-      <c r="I21" s="8" t="str">
+      <c r="I21" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
@@ -2183,22 +2192,22 @@
         <v>34</v>
       </c>
       <c r="L21" s="0"/>
-      <c r="M21" s="11" t="n">
+      <c r="M21" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N21" s="11" t="n">
+      <c r="N21" s="10" t="n">
         <f aca="false">N4</f>
         <v>2001</v>
       </c>
-      <c r="O21" s="11" t="n">
+      <c r="O21" s="10" t="n">
         <f aca="false">O5</f>
         <v>3031</v>
       </c>
       <c r="P21" s="0"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
@@ -2221,28 +2230,28 @@
         <v>7</v>
       </c>
       <c r="H22" s="7"/>
-      <c r="I22" s="8" t="str">
+      <c r="I22" s="6" t="str">
         <f aca="false">$I$3</f>
         <v>Déchets - Propreté publique</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="12" t="s">
         <v>31</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="11" t="n">
+      <c r="M22" s="10" t="n">
         <f aca="false">$M$3</f>
         <v>1002</v>
       </c>
-      <c r="N22" s="11" t="n">
+      <c r="N22" s="10" t="n">
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O22" s="11" t="n">
+      <c r="O22" s="10" t="n">
         <f aca="false">O6</f>
         <v>3032</v>
       </c>
@@ -2288,14 +2297,14 @@
         <v>48</v>
       </c>
       <c r="L23" s="0"/>
-      <c r="M23" s="9" t="n">
+      <c r="M23" s="8" t="n">
         <f aca="false">E23+1000</f>
         <v>1006</v>
       </c>
-      <c r="N23" s="9" t="n">
+      <c r="N23" s="8" t="n">
         <v>2010</v>
       </c>
-      <c r="O23" s="9" t="n">
+      <c r="O23" s="8" t="n">
         <f aca="false">G23+3000</f>
         <v>3126</v>
       </c>
@@ -2336,10 +2345,10 @@
         <f aca="false">$M$23</f>
         <v>1006</v>
       </c>
-      <c r="N24" s="9" t="n">
+      <c r="N24" s="8" t="n">
         <v>2011</v>
       </c>
-      <c r="O24" s="9" t="n">
+      <c r="O24" s="8" t="n">
         <f aca="false">G24+3000</f>
         <v>3127</v>
       </c>
@@ -2380,10 +2389,10 @@
         <f aca="false">$M$23</f>
         <v>1006</v>
       </c>
-      <c r="N25" s="9" t="n">
+      <c r="N25" s="8" t="n">
         <v>2012</v>
       </c>
-      <c r="O25" s="9" t="n">
+      <c r="O25" s="8" t="n">
         <f aca="false">G25+3000</f>
         <v>3123</v>
       </c>
@@ -2428,7 +2437,7 @@
         <f aca="false">N23</f>
         <v>2010</v>
       </c>
-      <c r="O26" s="9" t="n">
+      <c r="O26" s="8" t="n">
         <f aca="false">G26+3000</f>
         <v>3044</v>
       </c>
@@ -2473,7 +2482,7 @@
         <f aca="false">N23</f>
         <v>2010</v>
       </c>
-      <c r="O27" s="9" t="n">
+      <c r="O27" s="8" t="n">
         <f aca="false">G27+3000</f>
         <v>3043</v>
       </c>
@@ -2518,7 +2527,7 @@
         <f aca="false">N24</f>
         <v>2011</v>
       </c>
-      <c r="O28" s="9" t="n">
+      <c r="O28" s="8" t="n">
         <f aca="false">G28+3000</f>
         <v>3042</v>
       </c>
@@ -2563,7 +2572,7 @@
         <f aca="false">N23</f>
         <v>2010</v>
       </c>
-      <c r="O29" s="9" t="n">
+      <c r="O29" s="8" t="n">
         <f aca="false">G29+3000</f>
         <v>3124</v>
       </c>
@@ -2608,7 +2617,7 @@
         <f aca="false">N25</f>
         <v>2012</v>
       </c>
-      <c r="O30" s="9" t="n">
+      <c r="O30" s="8" t="n">
         <f aca="false">G30+3000</f>
         <v>3125</v>
       </c>
@@ -4066,14 +4075,14 @@
         <v>67</v>
       </c>
       <c r="L63" s="0"/>
-      <c r="M63" s="9" t="n">
+      <c r="M63" s="8" t="n">
         <f aca="false">E63+1000</f>
         <v>1008</v>
       </c>
-      <c r="N63" s="9" t="n">
+      <c r="N63" s="8" t="n">
         <v>2020</v>
       </c>
-      <c r="O63" s="9" t="n">
+      <c r="O63" s="8" t="n">
         <f aca="false">G63+3000</f>
         <v>3049</v>
       </c>
@@ -4159,10 +4168,10 @@
         <f aca="false">$M$63</f>
         <v>1008</v>
       </c>
-      <c r="N65" s="9" t="n">
+      <c r="N65" s="8" t="n">
         <v>2021</v>
       </c>
-      <c r="O65" s="9" t="n">
+      <c r="O65" s="8" t="n">
         <f aca="false">G65+3000</f>
         <v>3048</v>
       </c>
@@ -4467,14 +4476,14 @@
         <v>75</v>
       </c>
       <c r="L72" s="0"/>
-      <c r="M72" s="9" t="n">
+      <c r="M72" s="8" t="n">
         <f aca="false">E72+1000</f>
         <v>1007</v>
       </c>
-      <c r="N72" s="9" t="n">
+      <c r="N72" s="8" t="n">
         <v>2030</v>
       </c>
-      <c r="O72" s="9" t="n">
+      <c r="O72" s="8" t="n">
         <f aca="false">G72+3000</f>
         <v>3045</v>
       </c>
@@ -4519,7 +4528,7 @@
         <f aca="false">$N$72</f>
         <v>2030</v>
       </c>
-      <c r="O73" s="9" t="n">
+      <c r="O73" s="8" t="n">
         <f aca="false">G73+3000</f>
         <v>3046</v>
       </c>
@@ -5137,18 +5146,18 @@
       <c r="J87" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K87" s="14" t="s">
+      <c r="K87" s="13" t="s">
         <v>82</v>
       </c>
       <c r="L87" s="0"/>
-      <c r="M87" s="9" t="n">
+      <c r="M87" s="8" t="n">
         <f aca="false">E87+1000</f>
         <v>1004</v>
       </c>
-      <c r="N87" s="9" t="n">
+      <c r="N87" s="8" t="n">
         <v>2040</v>
       </c>
-      <c r="O87" s="9" t="n">
+      <c r="O87" s="8" t="n">
         <f aca="false">G87+3000</f>
         <v>3035</v>
       </c>
@@ -5181,7 +5190,7 @@
       <c r="J88" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K88" s="14" t="s">
+      <c r="K88" s="13" t="s">
         <v>84</v>
       </c>
       <c r="L88" s="0"/>
@@ -5189,10 +5198,10 @@
         <f aca="false">$M$87</f>
         <v>1004</v>
       </c>
-      <c r="N88" s="9" t="n">
+      <c r="N88" s="8" t="n">
         <v>2041</v>
       </c>
-      <c r="O88" s="9" t="n">
+      <c r="O88" s="8" t="n">
         <f aca="false">G88+3000</f>
         <v>3036</v>
       </c>
@@ -5225,7 +5234,7 @@
       <c r="J89" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K89" s="14" t="s">
+      <c r="K89" s="13" t="s">
         <v>86</v>
       </c>
       <c r="L89" s="0"/>
@@ -5233,10 +5242,10 @@
         <f aca="false">$M$87</f>
         <v>1004</v>
       </c>
-      <c r="N89" s="9" t="n">
+      <c r="N89" s="8" t="n">
         <v>2042</v>
       </c>
-      <c r="O89" s="9" t="n">
+      <c r="O89" s="8" t="n">
         <f aca="false">G89+3000</f>
         <v>3037</v>
       </c>
@@ -5269,7 +5278,7 @@
       <c r="J90" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K90" s="14" t="s">
+      <c r="K90" s="13" t="s">
         <v>87</v>
       </c>
       <c r="L90" s="0"/>
@@ -5314,7 +5323,7 @@
       <c r="J91" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K91" s="14" t="s">
+      <c r="K91" s="13" t="s">
         <v>84</v>
       </c>
       <c r="L91" s="0"/>
@@ -5359,7 +5368,7 @@
       <c r="J92" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K92" s="14" t="s">
+      <c r="K92" s="13" t="s">
         <v>86</v>
       </c>
       <c r="L92" s="0"/>
@@ -5404,7 +5413,7 @@
       <c r="J93" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K93" s="14" t="s">
+      <c r="K93" s="13" t="s">
         <v>84</v>
       </c>
       <c r="L93" s="0"/>
@@ -5449,7 +5458,7 @@
       <c r="J94" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K94" s="14" t="s">
+      <c r="K94" s="13" t="s">
         <v>86</v>
       </c>
       <c r="L94" s="0"/>
@@ -5494,7 +5503,7 @@
       <c r="J95" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K95" s="14" t="s">
+      <c r="K95" s="13" t="s">
         <v>87</v>
       </c>
       <c r="L95" s="0"/>
@@ -5539,7 +5548,7 @@
       <c r="J96" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K96" s="14" t="s">
+      <c r="K96" s="13" t="s">
         <v>86</v>
       </c>
       <c r="L96" s="0"/>
@@ -5584,7 +5593,7 @@
       <c r="J97" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K97" s="14" t="s">
+      <c r="K97" s="13" t="s">
         <v>87</v>
       </c>
       <c r="L97" s="0"/>
@@ -5629,7 +5638,7 @@
       <c r="J98" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K98" s="14" t="s">
+      <c r="K98" s="13" t="s">
         <v>84</v>
       </c>
       <c r="L98" s="0"/>
@@ -5671,21 +5680,21 @@
       <c r="I99" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J99" s="15" t="s">
+      <c r="J99" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K99" s="16" t="s">
+      <c r="K99" s="15" t="s">
         <v>91</v>
       </c>
       <c r="L99" s="0"/>
-      <c r="M99" s="9" t="n">
+      <c r="M99" s="8" t="n">
         <f aca="false">E99+1000</f>
         <v>1003</v>
       </c>
-      <c r="N99" s="9" t="n">
+      <c r="N99" s="8" t="n">
         <v>2050</v>
       </c>
-      <c r="O99" s="9" t="n">
+      <c r="O99" s="8" t="n">
         <f aca="false">G99+3000</f>
         <v>3033</v>
       </c>
@@ -5718,7 +5727,7 @@
       <c r="J100" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K100" s="14" t="s">
+      <c r="K100" s="13" t="s">
         <v>92</v>
       </c>
       <c r="L100" s="0"/>
@@ -5726,10 +5735,10 @@
         <f aca="false">$M$99</f>
         <v>1003</v>
       </c>
-      <c r="N100" s="9" t="n">
+      <c r="N100" s="8" t="n">
         <v>2051</v>
       </c>
-      <c r="O100" s="9" t="n">
+      <c r="O100" s="8" t="n">
         <f aca="false">G100+3000</f>
         <v>3034</v>
       </c>
@@ -5762,17 +5771,17 @@
       <c r="J101" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K101" s="14" t="s">
+      <c r="K101" s="13" t="s">
         <v>95</v>
       </c>
       <c r="L101" s="0"/>
-      <c r="M101" s="9" t="n">
+      <c r="M101" s="8" t="n">
         <v>1010</v>
       </c>
-      <c r="N101" s="9" t="n">
+      <c r="N101" s="8" t="n">
         <v>2052</v>
       </c>
-      <c r="O101" s="9" t="n">
+      <c r="O101" s="8" t="n">
         <f aca="false">G101+3000</f>
         <v>3117</v>
       </c>
@@ -5802,10 +5811,10 @@
       <c r="I102" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J102" s="15" t="s">
+      <c r="J102" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K102" s="16" t="s">
+      <c r="K102" s="15" t="s">
         <v>91</v>
       </c>
       <c r="L102" s="0"/>
@@ -5850,7 +5859,7 @@
       <c r="J103" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K103" s="14" t="s">
+      <c r="K103" s="13" t="s">
         <v>92</v>
       </c>
       <c r="L103" s="0"/>
@@ -5892,10 +5901,10 @@
       <c r="I104" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J104" s="15" t="s">
+      <c r="J104" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K104" s="16" t="s">
+      <c r="K104" s="15" t="s">
         <v>91</v>
       </c>
       <c r="L104" s="0"/>
@@ -5940,7 +5949,7 @@
       <c r="J105" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K105" s="14" t="s">
+      <c r="K105" s="13" t="s">
         <v>92</v>
       </c>
       <c r="L105" s="0"/>
@@ -5982,10 +5991,10 @@
       <c r="I106" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J106" s="15" t="s">
+      <c r="J106" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K106" s="16" t="s">
+      <c r="K106" s="15" t="s">
         <v>91</v>
       </c>
       <c r="L106" s="0"/>
@@ -6030,7 +6039,7 @@
       <c r="J107" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K107" s="14" t="s">
+      <c r="K107" s="13" t="s">
         <v>92</v>
       </c>
       <c r="L107" s="0"/>
@@ -6072,10 +6081,10 @@
       <c r="I108" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J108" s="15" t="s">
+      <c r="J108" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K108" s="16" t="s">
+      <c r="K108" s="15" t="s">
         <v>91</v>
       </c>
       <c r="L108" s="0"/>
@@ -6120,7 +6129,7 @@
       <c r="J109" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K109" s="14" t="s">
+      <c r="K109" s="13" t="s">
         <v>92</v>
       </c>
       <c r="L109" s="0"/>
@@ -6165,18 +6174,18 @@
       <c r="J110" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K110" s="14" t="s">
+      <c r="K110" s="13" t="s">
         <v>99</v>
       </c>
       <c r="L110" s="0"/>
-      <c r="M110" s="9" t="n">
+      <c r="M110" s="8" t="n">
         <f aca="false">E110+1000</f>
         <v>1001</v>
       </c>
-      <c r="N110" s="9" t="n">
+      <c r="N110" s="8" t="n">
         <v>2060</v>
       </c>
-      <c r="O110" s="9" t="n">
+      <c r="O110" s="8" t="n">
         <f aca="false">G110+3000</f>
         <v>3026</v>
       </c>
@@ -6209,7 +6218,7 @@
       <c r="J111" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K111" s="14" t="s">
+      <c r="K111" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L111" s="0"/>
@@ -6217,10 +6226,10 @@
         <f aca="false">$M$110</f>
         <v>1001</v>
       </c>
-      <c r="N111" s="9" t="n">
+      <c r="N111" s="8" t="n">
         <v>2061</v>
       </c>
-      <c r="O111" s="9" t="n">
+      <c r="O111" s="8" t="n">
         <f aca="false">G111+3000</f>
         <v>3027</v>
       </c>
@@ -6253,7 +6262,7 @@
       <c r="J112" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K112" s="14" t="s">
+      <c r="K112" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L112" s="0"/>
@@ -6298,7 +6307,7 @@
       <c r="J113" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K113" s="14" t="s">
+      <c r="K113" s="13" t="s">
         <v>99</v>
       </c>
       <c r="L113" s="0"/>
@@ -6343,7 +6352,7 @@
       <c r="J114" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K114" s="14" t="s">
+      <c r="K114" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L114" s="0"/>
@@ -6388,7 +6397,7 @@
       <c r="J115" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K115" s="14" t="s">
+      <c r="K115" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L115" s="0"/>
@@ -6433,7 +6442,7 @@
       <c r="J116" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K116" s="14" t="s">
+      <c r="K116" s="13" t="s">
         <v>99</v>
       </c>
       <c r="L116" s="0"/>
@@ -6478,7 +6487,7 @@
       <c r="J117" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K117" s="14" t="s">
+      <c r="K117" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L117" s="0"/>
@@ -6523,7 +6532,7 @@
       <c r="J118" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K118" s="14" t="s">
+      <c r="K118" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L118" s="0"/>
@@ -6568,7 +6577,7 @@
       <c r="J119" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K119" s="14" t="s">
+      <c r="K119" s="13" t="s">
         <v>99</v>
       </c>
       <c r="L119" s="0"/>
@@ -6613,7 +6622,7 @@
       <c r="J120" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K120" s="14" t="s">
+      <c r="K120" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L120" s="0"/>
@@ -6658,7 +6667,7 @@
       <c r="J121" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K121" s="14" t="s">
+      <c r="K121" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L121" s="0"/>
@@ -6703,7 +6712,7 @@
       <c r="J122" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K122" s="14" t="s">
+      <c r="K122" s="13" t="s">
         <v>99</v>
       </c>
       <c r="L122" s="0"/>
@@ -6748,7 +6757,7 @@
       <c r="J123" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K123" s="14" t="s">
+      <c r="K123" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L123" s="0"/>
@@ -6793,7 +6802,7 @@
       <c r="J124" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K124" s="14" t="s">
+      <c r="K124" s="13" t="s">
         <v>101</v>
       </c>
       <c r="L124" s="0"/>
@@ -6838,18 +6847,18 @@
       <c r="J125" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K125" s="14" t="s">
+      <c r="K125" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L125" s="0"/>
-      <c r="M125" s="9" t="n">
+      <c r="M125" s="8" t="n">
         <f aca="false">E125+1000</f>
         <v>1005</v>
       </c>
-      <c r="N125" s="9" t="n">
+      <c r="N125" s="8" t="n">
         <v>2070</v>
       </c>
-      <c r="O125" s="9" t="n">
+      <c r="O125" s="8" t="n">
         <f aca="false">G125+3000</f>
         <v>3038</v>
       </c>
@@ -6882,7 +6891,7 @@
       <c r="J126" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K126" s="14" t="s">
+      <c r="K126" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L126" s="0"/>
@@ -6927,7 +6936,7 @@
       <c r="J127" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K127" s="14" t="s">
+      <c r="K127" s="13" t="s">
         <v>108</v>
       </c>
       <c r="L127" s="0"/>
@@ -6935,10 +6944,10 @@
         <f aca="false">M125</f>
         <v>1005</v>
       </c>
-      <c r="N127" s="9" t="n">
+      <c r="N127" s="8" t="n">
         <v>2071</v>
       </c>
-      <c r="O127" s="9" t="n">
+      <c r="O127" s="8" t="n">
         <f aca="false">G127+3000</f>
         <v>3041</v>
       </c>
@@ -6971,7 +6980,7 @@
       <c r="J128" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K128" s="14" t="s">
+      <c r="K128" s="13" t="s">
         <v>110</v>
       </c>
       <c r="L128" s="0"/>
@@ -6979,10 +6988,10 @@
         <f aca="false">M110</f>
         <v>1001</v>
       </c>
-      <c r="N128" s="9" t="n">
+      <c r="N128" s="8" t="n">
         <v>2072</v>
       </c>
-      <c r="O128" s="9" t="n">
+      <c r="O128" s="8" t="n">
         <f aca="false">G128+3000</f>
         <v>3040</v>
       </c>
@@ -7015,7 +7024,7 @@
       <c r="J129" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K129" s="14" t="s">
+      <c r="K129" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L129" s="0"/>
@@ -7060,7 +7069,7 @@
       <c r="J130" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K130" s="14" t="s">
+      <c r="K130" s="13" t="s">
         <v>110</v>
       </c>
       <c r="L130" s="0"/>
@@ -7105,7 +7114,7 @@
       <c r="J131" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K131" s="14" t="s">
+      <c r="K131" s="13" t="s">
         <v>108</v>
       </c>
       <c r="L131" s="0"/>
@@ -7150,7 +7159,7 @@
       <c r="J132" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K132" s="14" t="s">
+      <c r="K132" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L132" s="0"/>
@@ -7195,7 +7204,7 @@
       <c r="J133" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K133" s="14" t="s">
+      <c r="K133" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L133" s="0"/>
@@ -7240,7 +7249,7 @@
       <c r="J134" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K134" s="14" t="s">
+      <c r="K134" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L134" s="0"/>
@@ -7285,7 +7294,7 @@
       <c r="J135" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K135" s="14" t="s">
+      <c r="K135" s="13" t="s">
         <v>108</v>
       </c>
       <c r="L135" s="0"/>
@@ -7330,7 +7339,7 @@
       <c r="J136" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K136" s="14" t="s">
+      <c r="K136" s="13" t="s">
         <v>110</v>
       </c>
       <c r="L136" s="0"/>
@@ -7375,7 +7384,7 @@
       <c r="J137" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K137" s="14" t="s">
+      <c r="K137" s="13" t="s">
         <v>108</v>
       </c>
       <c r="L137" s="0"/>
@@ -7420,7 +7429,7 @@
       <c r="J138" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K138" s="14" t="s">
+      <c r="K138" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L138" s="0"/>
@@ -7465,7 +7474,7 @@
       <c r="J139" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K139" s="14" t="s">
+      <c r="K139" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L139" s="0"/>
@@ -7510,7 +7519,7 @@
       <c r="J140" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K140" s="14" t="s">
+      <c r="K140" s="13" t="s">
         <v>110</v>
       </c>
       <c r="L140" s="0"/>
@@ -7555,7 +7564,7 @@
       <c r="J141" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K141" s="14" t="s">
+      <c r="K141" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L141" s="0"/>
@@ -7600,7 +7609,7 @@
       <c r="J142" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K142" s="14" t="s">
+      <c r="K142" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L142" s="0"/>
@@ -7645,7 +7654,7 @@
       <c r="J143" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K143" s="14" t="s">
+      <c r="K143" s="13" t="s">
         <v>108</v>
       </c>
       <c r="L143" s="0"/>
@@ -7690,7 +7699,7 @@
       <c r="J144" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K144" s="14" t="s">
+      <c r="K144" s="13" t="s">
         <v>110</v>
       </c>
       <c r="L144" s="0"/>
@@ -7743,10 +7752,10 @@
         <f aca="false">M72</f>
         <v>1007</v>
       </c>
-      <c r="N145" s="9" t="n">
+      <c r="N145" s="8" t="n">
         <v>2200</v>
       </c>
-      <c r="O145" s="9" t="n">
+      <c r="O145" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="P145" s="0"/>
@@ -7796,7 +7805,7 @@
         <f aca="false">N145</f>
         <v>2200</v>
       </c>
-      <c r="O146" s="9" t="n">
+      <c r="O146" s="8" t="n">
         <v>3301</v>
       </c>
       <c r="P146" s="0"/>
@@ -7944,10 +7953,10 @@
         <f aca="false">M99</f>
         <v>1003</v>
       </c>
-      <c r="N149" s="9" t="n">
+      <c r="N149" s="8" t="n">
         <v>2201</v>
       </c>
-      <c r="O149" s="9" t="n">
+      <c r="O149" s="8" t="n">
         <v>3302</v>
       </c>
       <c r="P149" s="0"/>
@@ -7985,7 +7994,7 @@
       <c r="J150" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K150" s="15" t="s">
+      <c r="K150" s="14" t="s">
         <v>91</v>
       </c>
       <c r="L150" s="0"/>
@@ -8049,7 +8058,7 @@
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O151" s="9" t="n">
+      <c r="O151" s="8" t="n">
         <v>3304</v>
       </c>
       <c r="P151" s="0"/>
@@ -8100,14 +8109,14 @@
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O152" s="9" t="n">
+      <c r="O152" s="8" t="n">
         <v>3305</v>
       </c>
       <c r="P152" s="0"/>
-      <c r="Q152" s="0" t="n">
+      <c r="Q152" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R152" s="0" t="n">
+      <c r="R152" s="16" t="n">
         <v>68</v>
       </c>
     </row>
@@ -8146,13 +8155,19 @@
         <f aca="false">M110</f>
         <v>1001</v>
       </c>
-      <c r="N153" s="9" t="n">
+      <c r="N153" s="8" t="n">
         <v>2203</v>
       </c>
-      <c r="O153" s="9" t="n">
+      <c r="O153" s="8" t="n">
         <v>3306</v>
       </c>
       <c r="P153" s="0"/>
+      <c r="Q153" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="R153" s="16" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
@@ -8194,14 +8209,14 @@
         <f aca="false">N6</f>
         <v>2002</v>
       </c>
-      <c r="O154" s="9" t="n">
+      <c r="O154" s="8" t="n">
         <v>3307</v>
       </c>
       <c r="P154" s="0"/>
-      <c r="Q154" s="0" t="n">
+      <c r="Q154" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R154" s="0" t="n">
+      <c r="R154" s="16" t="n">
         <v>19</v>
       </c>
     </row>
@@ -8250,10 +8265,10 @@
         <v>3030</v>
       </c>
       <c r="P155" s="0"/>
-      <c r="Q155" s="0" t="n">
+      <c r="Q155" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R155" s="0" t="n">
+      <c r="R155" s="16" t="n">
         <v>18</v>
       </c>
     </row>
@@ -8304,10 +8319,10 @@
         <v>3032</v>
       </c>
       <c r="P156" s="0"/>
-      <c r="Q156" s="0" t="n">
+      <c r="Q156" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R156" s="0" t="n">
+      <c r="R156" s="16" t="n">
         <v>17</v>
       </c>
     </row>
@@ -8361,10 +8376,10 @@
         <f aca="false">P6</f>
         <v>4010</v>
       </c>
-      <c r="Q157" s="0" t="n">
+      <c r="Q157" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R157" s="0" t="n">
+      <c r="R157" s="16" t="n">
         <v>16</v>
       </c>
     </row>
@@ -8412,13 +8427,13 @@
         <f aca="false">O151</f>
         <v>3304</v>
       </c>
-      <c r="P158" s="9" t="n">
+      <c r="P158" s="8" t="n">
         <v>4011</v>
       </c>
-      <c r="Q158" s="0" t="n">
+      <c r="Q158" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R158" s="0" t="n">
+      <c r="R158" s="16" t="n">
         <v>78</v>
       </c>
     </row>
@@ -8467,10 +8482,10 @@
         <v>3305</v>
       </c>
       <c r="P159" s="0"/>
-      <c r="Q159" s="0" t="n">
+      <c r="Q159" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R159" s="0" t="n">
+      <c r="R159" s="16" t="n">
         <v>68</v>
       </c>
     </row>
@@ -8518,6 +8533,12 @@
         <v>3306</v>
       </c>
       <c r="P160" s="0"/>
+      <c r="Q160" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="R160" s="16" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
@@ -8564,10 +8585,10 @@
         <v>3307</v>
       </c>
       <c r="P161" s="0"/>
-      <c r="Q161" s="0" t="n">
+      <c r="Q161" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R161" s="0" t="n">
+      <c r="R161" s="16" t="n">
         <v>19</v>
       </c>
     </row>
@@ -8616,10 +8637,10 @@
         <v>3030</v>
       </c>
       <c r="P162" s="0"/>
-      <c r="Q162" s="0" t="n">
+      <c r="Q162" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="R162" s="0" t="n">
+      <c r="R162" s="16" t="n">
         <v>18</v>
       </c>
     </row>
@@ -8772,10 +8793,10 @@
         <f aca="false">M72</f>
         <v>1007</v>
       </c>
-      <c r="N165" s="9" t="n">
+      <c r="N165" s="8" t="n">
         <v>2204</v>
       </c>
-      <c r="O165" s="9" t="n">
+      <c r="O165" s="8" t="n">
         <v>3310</v>
       </c>
       <c r="P165" s="0"/>
@@ -8825,7 +8846,7 @@
         <f aca="false">$N$165</f>
         <v>2204</v>
       </c>
-      <c r="O166" s="9" t="n">
+      <c r="O166" s="8" t="n">
         <v>3311</v>
       </c>
       <c r="P166" s="0"/>
@@ -8875,7 +8896,7 @@
         <f aca="false">$N$165</f>
         <v>2204</v>
       </c>
-      <c r="O167" s="9" t="n">
+      <c r="O167" s="8" t="n">
         <v>3312</v>
       </c>
       <c r="P167" s="0"/>
@@ -8925,7 +8946,7 @@
         <f aca="false">$N$165</f>
         <v>2204</v>
       </c>
-      <c r="O168" s="9" t="n">
+      <c r="O168" s="8" t="n">
         <v>3313</v>
       </c>
       <c r="P168" s="0"/>
@@ -9191,7 +9212,7 @@
         <f aca="false">$O$3</f>
         <v>3029</v>
       </c>
-      <c r="P173" s="9" t="n">
+      <c r="P173" s="8" t="n">
         <f aca="false">H173+4000</f>
         <v>4001</v>
       </c>
@@ -9258,7 +9279,7 @@
         <f aca="false">$O$3</f>
         <v>3029</v>
       </c>
-      <c r="P174" s="9" t="n">
+      <c r="P174" s="8" t="n">
         <f aca="false">H174+4000</f>
         <v>4002</v>
       </c>
@@ -9325,7 +9346,7 @@
         <f aca="false">$O$3</f>
         <v>3029</v>
       </c>
-      <c r="P175" s="9" t="n">
+      <c r="P175" s="8" t="n">
         <f aca="false">H175+4000</f>
         <v>4003</v>
       </c>
@@ -9392,7 +9413,7 @@
         <f aca="false">$O$3</f>
         <v>3029</v>
       </c>
-      <c r="P176" s="9" t="n">
+      <c r="P176" s="8" t="n">
         <f aca="false">H176+4000</f>
         <v>4004</v>
       </c>
@@ -9459,7 +9480,7 @@
         <f aca="false">$O$3</f>
         <v>3029</v>
       </c>
-      <c r="P177" s="9" t="n">
+      <c r="P177" s="8" t="n">
         <f aca="false">H177+4000</f>
         <v>4005</v>
       </c>
@@ -9526,7 +9547,7 @@
         <f aca="false">$O$3</f>
         <v>3029</v>
       </c>
-      <c r="P178" s="9" t="n">
+      <c r="P178" s="8" t="n">
         <f aca="false">H178+4000</f>
         <v>4006</v>
       </c>
@@ -9987,7 +10008,7 @@
         <f aca="false">$N$3</f>
         <v>2000</v>
       </c>
-      <c r="O185" s="9" t="n">
+      <c r="O185" s="8" t="n">
         <v>3314</v>
       </c>
       <c r="P185" s="2" t="n">
@@ -11561,25 +11582,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6477732793522"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.1457489878543"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6113360323887"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="8.19028340080972"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.7449392712551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.4736842105263"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11631,6 +11656,19 @@
       <c r="P1" s="17" t="s">
         <v>177</v>
       </c>
+      <c r="Q1" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -11640,27 +11678,27 @@
         <v>96</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="M2" s="18" t="n">
+        <v>186</v>
+      </c>
+      <c r="M2" s="0" t="n">
         <f aca="false">mapping!M110</f>
         <v>1001</v>
       </c>
@@ -11670,7 +11708,10 @@
       <c r="O2" s="19" t="n">
         <v>3400</v>
       </c>
-      <c r="P2" s="18"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -11680,25 +11721,25 @@
         <v>27</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M3" s="0" t="n">
         <f aca="false">mapping!M125</f>
@@ -11710,6 +11751,10 @@
       <c r="O3" s="19" t="n">
         <v>3401</v>
       </c>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -11719,25 +11764,25 @@
         <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M4" s="0" t="n">
         <f aca="false">M3</f>
@@ -11749,6 +11794,10 @@
       <c r="O4" s="19" t="n">
         <v>3402</v>
       </c>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -11758,25 +11807,25 @@
         <v>81</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="M5" s="0" t="n">
         <f aca="false">mapping!M87</f>
@@ -11788,6 +11837,7 @@
       <c r="O5" s="19" t="n">
         <v>3403</v>
       </c>
+      <c r="T5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -11797,25 +11847,25 @@
         <v>81</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M6" s="0" t="n">
         <f aca="false">M5</f>
@@ -11827,6 +11877,16 @@
       <c r="O6" s="19" t="n">
         <v>3404</v>
       </c>
+      <c r="Q6" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="R6" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="S6" s="16" t="n">
+        <v>78</v>
+      </c>
+      <c r="T6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -11836,25 +11896,25 @@
         <v>94</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M7" s="0" t="n">
         <f aca="false">mapping!M101</f>
@@ -11866,6 +11926,10 @@
       <c r="O7" s="19" t="n">
         <v>3405</v>
       </c>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -11875,25 +11939,25 @@
         <v>73</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M8" s="0" t="n">
         <f aca="false">mapping!M72</f>
@@ -11905,6 +11969,10 @@
       <c r="O8" s="19" t="n">
         <v>3406</v>
       </c>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -11914,25 +11982,25 @@
         <v>73</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="M9" s="0" t="n">
         <f aca="false">M8</f>
@@ -11944,6 +12012,9 @@
       <c r="O9" s="19" t="n">
         <v>3407</v>
       </c>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -11953,25 +12024,25 @@
         <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="M10" s="0" t="n">
         <f aca="false">mapping!M23</f>
@@ -11984,6 +12055,12 @@
       <c r="O10" s="19" t="n">
         <v>3408</v>
       </c>
+      <c r="Q10" s="16" t="n">
+        <v>143</v>
+      </c>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -11993,25 +12070,25 @@
         <v>66</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="M11" s="0" t="n">
         <f aca="false">mapping!M63</f>
@@ -12023,6 +12100,10 @@
       <c r="O11" s="19" t="n">
         <v>3409</v>
       </c>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -12032,25 +12113,25 @@
         <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="M12" s="0" t="n">
         <f aca="false">M11</f>
@@ -12062,83 +12143,95 @@
       <c r="O12" s="19" t="n">
         <v>3410</v>
       </c>
-    </row>
-    <row r="13" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D13" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>2311</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>3411</v>
+      </c>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="G14" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="M13" s="18" t="n">
-        <v>1100</v>
-      </c>
-      <c r="N13" s="18" t="n">
-        <v>2311</v>
-      </c>
-      <c r="O13" s="18" t="n">
-        <v>3411</v>
-      </c>
-    </row>
-    <row r="14" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="M14" s="18" t="n">
+      <c r="M14" s="0" t="n">
         <f aca="false">M13</f>
         <v>1100</v>
       </c>
-      <c r="N14" s="18" t="n">
+      <c r="N14" s="0" t="n">
         <v>2312</v>
       </c>
-      <c r="O14" s="18" t="n">
+      <c r="O14" s="0" t="n">
         <v>3412</v>
       </c>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
FMX-1029: Fix problem of offset in mapping.
</commit_message>
<xml_diff>
--- a/apps/resources/categories_mapping_new.xlsx
+++ b/apps/resources/categories_mapping_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,6 +46,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">mapping!$1:$2</definedName>
@@ -53,6 +54,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
@@ -60,6 +62,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -902,7 +905,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -967,12 +970,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1071,30 +1070,30 @@
   </sheetPr>
   <dimension ref="1:208"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S26" activeCellId="0" sqref="S26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I185" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P164" activeCellId="0" sqref="P164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.2429149797571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.57085020242915"/>
   </cols>
@@ -8113,10 +8112,10 @@
         <v>3305</v>
       </c>
       <c r="P152" s="0"/>
-      <c r="Q152" s="16" t="n">
+      <c r="Q152" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R152" s="16" t="n">
+      <c r="R152" s="0" t="n">
         <v>68</v>
       </c>
     </row>
@@ -8162,10 +8161,10 @@
         <v>3306</v>
       </c>
       <c r="P153" s="0"/>
-      <c r="Q153" s="16" t="n">
+      <c r="Q153" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R153" s="16" t="n">
+      <c r="R153" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -8213,10 +8212,10 @@
         <v>3307</v>
       </c>
       <c r="P154" s="0"/>
-      <c r="Q154" s="16" t="n">
+      <c r="Q154" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R154" s="16" t="n">
+      <c r="R154" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -8265,10 +8264,10 @@
         <v>3030</v>
       </c>
       <c r="P155" s="0"/>
-      <c r="Q155" s="16" t="n">
+      <c r="Q155" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R155" s="16" t="n">
+      <c r="R155" s="0" t="n">
         <v>18</v>
       </c>
     </row>
@@ -8318,11 +8317,13 @@
         <f aca="false">O6</f>
         <v>3032</v>
       </c>
-      <c r="P156" s="0"/>
-      <c r="Q156" s="16" t="n">
+      <c r="P156" s="8" t="n">
+        <v>4011</v>
+      </c>
+      <c r="Q156" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R156" s="16" t="n">
+      <c r="R156" s="0" t="n">
         <v>17</v>
       </c>
     </row>
@@ -8372,14 +8373,14 @@
         <f aca="false">O6</f>
         <v>3032</v>
       </c>
-      <c r="P157" s="2" t="n">
+      <c r="P157" s="16" t="n">
         <f aca="false">P6</f>
         <v>4010</v>
       </c>
-      <c r="Q157" s="16" t="n">
+      <c r="Q157" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R157" s="16" t="n">
+      <c r="R157" s="0" t="n">
         <v>16</v>
       </c>
     </row>
@@ -8427,13 +8428,11 @@
         <f aca="false">O151</f>
         <v>3304</v>
       </c>
-      <c r="P158" s="8" t="n">
-        <v>4011</v>
-      </c>
-      <c r="Q158" s="16" t="n">
+      <c r="P158" s="0"/>
+      <c r="Q158" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R158" s="16" t="n">
+      <c r="R158" s="0" t="n">
         <v>78</v>
       </c>
     </row>
@@ -8482,10 +8481,10 @@
         <v>3305</v>
       </c>
       <c r="P159" s="0"/>
-      <c r="Q159" s="16" t="n">
+      <c r="Q159" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R159" s="16" t="n">
+      <c r="R159" s="0" t="n">
         <v>68</v>
       </c>
     </row>
@@ -8533,10 +8532,10 @@
         <v>3306</v>
       </c>
       <c r="P160" s="0"/>
-      <c r="Q160" s="16" t="n">
+      <c r="Q160" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R160" s="16" t="n">
+      <c r="R160" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -8585,10 +8584,10 @@
         <v>3307</v>
       </c>
       <c r="P161" s="0"/>
-      <c r="Q161" s="16" t="n">
+      <c r="Q161" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R161" s="16" t="n">
+      <c r="R161" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -8637,10 +8636,10 @@
         <v>3030</v>
       </c>
       <c r="P162" s="0"/>
-      <c r="Q162" s="16" t="n">
+      <c r="Q162" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R162" s="16" t="n">
+      <c r="R162" s="0" t="n">
         <v>18</v>
       </c>
     </row>
@@ -8691,7 +8690,7 @@
         <v>3032</v>
       </c>
       <c r="P163" s="2" t="n">
-        <f aca="false">P158</f>
+        <f aca="false">P156</f>
         <v>4011</v>
       </c>
       <c r="Q163" s="0" t="n">
@@ -11584,26 +11583,26 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0323886639676"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="16" min="14" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.7449392712551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.4736842105263"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -11656,7 +11655,7 @@
       <c r="P1" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="17" t="s">
         <v>178</v>
       </c>
       <c r="R1" s="17" t="s">
@@ -11702,16 +11701,12 @@
         <f aca="false">mapping!M110</f>
         <v>1001</v>
       </c>
-      <c r="N2" s="19" t="n">
+      <c r="N2" s="18" t="n">
         <v>2300</v>
       </c>
-      <c r="O2" s="19" t="n">
+      <c r="O2" s="18" t="n">
         <v>3400</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -11745,16 +11740,12 @@
         <f aca="false">mapping!M125</f>
         <v>1005</v>
       </c>
-      <c r="N3" s="19" t="n">
+      <c r="N3" s="18" t="n">
         <v>2301</v>
       </c>
-      <c r="O3" s="19" t="n">
+      <c r="O3" s="18" t="n">
         <v>3401</v>
       </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -11788,16 +11779,12 @@
         <f aca="false">M3</f>
         <v>1005</v>
       </c>
-      <c r="N4" s="19" t="n">
+      <c r="N4" s="18" t="n">
         <v>2302</v>
       </c>
-      <c r="O4" s="19" t="n">
+      <c r="O4" s="18" t="n">
         <v>3402</v>
       </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -11831,13 +11818,12 @@
         <f aca="false">mapping!M87</f>
         <v>1004</v>
       </c>
-      <c r="N5" s="19" t="n">
+      <c r="N5" s="18" t="n">
         <v>2303</v>
       </c>
-      <c r="O5" s="19" t="n">
+      <c r="O5" s="18" t="n">
         <v>3403</v>
       </c>
-      <c r="T5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -11871,22 +11857,21 @@
         <f aca="false">M5</f>
         <v>1004</v>
       </c>
-      <c r="N6" s="19" t="n">
+      <c r="N6" s="18" t="n">
         <v>2304</v>
       </c>
-      <c r="O6" s="19" t="n">
+      <c r="O6" s="18" t="n">
         <v>3404</v>
       </c>
-      <c r="Q6" s="16" t="n">
+      <c r="Q6" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="R6" s="16" t="n">
+      <c r="R6" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="S6" s="16" t="n">
+      <c r="S6" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="T6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -11920,16 +11905,12 @@
         <f aca="false">mapping!M101</f>
         <v>1010</v>
       </c>
-      <c r="N7" s="19" t="n">
+      <c r="N7" s="18" t="n">
         <v>2305</v>
       </c>
-      <c r="O7" s="19" t="n">
+      <c r="O7" s="18" t="n">
         <v>3405</v>
       </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -11963,16 +11944,12 @@
         <f aca="false">mapping!M72</f>
         <v>1007</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="18" t="n">
         <v>2306</v>
       </c>
-      <c r="O8" s="19" t="n">
+      <c r="O8" s="18" t="n">
         <v>3406</v>
       </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -12006,15 +11983,12 @@
         <f aca="false">M8</f>
         <v>1007</v>
       </c>
-      <c r="N9" s="19" t="n">
+      <c r="N9" s="18" t="n">
         <v>2307</v>
       </c>
-      <c r="O9" s="19" t="n">
+      <c r="O9" s="18" t="n">
         <v>3407</v>
       </c>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -12052,15 +12026,12 @@
         <f aca="false">mapping!N25</f>
         <v>2012</v>
       </c>
-      <c r="O10" s="19" t="n">
+      <c r="O10" s="18" t="n">
         <v>3408</v>
       </c>
-      <c r="Q10" s="16" t="n">
+      <c r="Q10" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -12094,16 +12065,12 @@
         <f aca="false">mapping!M63</f>
         <v>1008</v>
       </c>
-      <c r="N11" s="19" t="n">
+      <c r="N11" s="18" t="n">
         <v>2308</v>
       </c>
-      <c r="O11" s="19" t="n">
+      <c r="O11" s="18" t="n">
         <v>3409</v>
       </c>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -12137,43 +12104,39 @@
         <f aca="false">M11</f>
         <v>1008</v>
       </c>
-      <c r="N12" s="19" t="n">
+      <c r="N12" s="18" t="n">
         <v>2309</v>
       </c>
-      <c r="O12" s="19" t="n">
+      <c r="O12" s="18" t="n">
         <v>3410</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>217</v>
       </c>
       <c r="M13" s="0" t="n">
@@ -12185,37 +12148,33 @@
       <c r="O13" s="0" t="n">
         <v>3411</v>
       </c>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>212</v>
       </c>
       <c r="M14" s="0" t="n">
@@ -12228,10 +12187,6 @@
       <c r="O14" s="0" t="n">
         <v>3412</v>
       </c>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
FMX-1086: New ABP fixtures and mappings from new typology
</commit_message>
<xml_diff>
--- a/apps/resources/categories_mapping_new.xlsx
+++ b/apps/resources/categories_mapping_new.xlsx
@@ -49,6 +49,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">mapping!$1:$2</definedName>
@@ -59,6 +61,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
@@ -69,6 +73,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -761,7 +767,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -806,12 +812,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -932,7 +932,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -997,7 +997,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1005,11 +1005,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1097,33 +1093,33 @@
   </sheetPr>
   <dimension ref="1:208"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H150" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U172" activeCellId="0" sqref="U172"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L154" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q167" activeCellId="0" sqref="Q167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.5263157894737"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.7449392712551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -11642,27 +11638,27 @@
   </sheetPr>
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S11" activeCellId="0" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="16" min="14" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.5384615384615"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12094,8 +12090,30 @@
       <c r="L10" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
+      <c r="M10" s="0" t="n">
+        <f aca="false">M9</f>
+        <v>1007</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">mapping!N165</f>
+        <v>2204</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">mapping!O167</f>
+        <v>3312</v>
+      </c>
+      <c r="P10" s="17" t="n">
+        <v>4050</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="U10" s="0" t="n">
         <v>9</v>
       </c>
@@ -12222,31 +12240,31 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="16" t="s">
         <v>222</v>
       </c>
       <c r="M14" s="0" t="n">
@@ -12260,31 +12278,31 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="16" t="s">
         <v>217</v>
       </c>
       <c r="M15" s="0" t="n">

</xml_diff>

<commit_message>
FMX-1028: Fix capital letter.
</commit_message>
<xml_diff>
--- a/apps/resources/categories_mapping_new.xlsx
+++ b/apps/resources/categories_mapping_new.xlsx
@@ -52,6 +52,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$1:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">mapping!$1:$2</definedName>
@@ -65,6 +66,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
@@ -78,6 +80,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">mapping!$A$2:$L$144</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -262,7 +265,7 @@
     <t xml:space="preserve"> Tronçon</t>
   </si>
   <si>
-    <t xml:space="preserve">éteinte</t>
+    <t xml:space="preserve">Éteinte</t>
   </si>
   <si>
     <t xml:space="preserve">Lampe allumée en continu</t>
@@ -773,7 +776,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -811,6 +814,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -934,11 +943,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -991,7 +1000,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1011,7 +1024,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1099,23 +1112,23 @@
   </sheetPr>
   <dimension ref="1:208"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q178" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V207" activeCellId="0" sqref="V207"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.17004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.3886639676113"/>
@@ -1123,9 +1136,9 @@
     <col collapsed="false" hidden="false" max="16" min="16" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="47.9109311740891"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="48.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2515,7 +2528,7 @@
       <c r="J27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K27" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L27" s="0"/>
@@ -2785,7 +2798,7 @@
       <c r="J33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="K33" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L33" s="0"/>
@@ -3010,7 +3023,7 @@
       <c r="J38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="K38" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L38" s="0"/>
@@ -3055,7 +3068,7 @@
       <c r="J39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="K39" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L39" s="0"/>
@@ -3279,7 +3292,7 @@
       <c r="J44" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="K44" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L44" s="0"/>
@@ -3457,7 +3470,7 @@
       <c r="J48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="K48" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L48" s="0"/>
@@ -3677,7 +3690,7 @@
       <c r="J53" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="K53" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L53" s="0"/>
@@ -3765,7 +3778,7 @@
       <c r="J55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="K55" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L55" s="0"/>
@@ -3984,7 +3997,7 @@
       <c r="J60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="K60" s="13" t="s">
         <v>57</v>
       </c>
       <c r="L60" s="0"/>
@@ -5191,7 +5204,7 @@
       <c r="J87" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K87" s="13" t="s">
+      <c r="K87" s="14" t="s">
         <v>85</v>
       </c>
       <c r="L87" s="0"/>
@@ -5235,7 +5248,7 @@
       <c r="J88" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K88" s="13" t="s">
+      <c r="K88" s="14" t="s">
         <v>87</v>
       </c>
       <c r="L88" s="0"/>
@@ -5279,7 +5292,7 @@
       <c r="J89" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K89" s="13" t="s">
+      <c r="K89" s="14" t="s">
         <v>89</v>
       </c>
       <c r="L89" s="0"/>
@@ -5323,7 +5336,7 @@
       <c r="J90" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K90" s="13" t="s">
+      <c r="K90" s="14" t="s">
         <v>90</v>
       </c>
       <c r="L90" s="0"/>
@@ -5368,7 +5381,7 @@
       <c r="J91" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K91" s="13" t="s">
+      <c r="K91" s="14" t="s">
         <v>87</v>
       </c>
       <c r="L91" s="0"/>
@@ -5413,7 +5426,7 @@
       <c r="J92" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K92" s="13" t="s">
+      <c r="K92" s="14" t="s">
         <v>89</v>
       </c>
       <c r="L92" s="0"/>
@@ -5458,7 +5471,7 @@
       <c r="J93" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K93" s="13" t="s">
+      <c r="K93" s="14" t="s">
         <v>87</v>
       </c>
       <c r="L93" s="0"/>
@@ -5503,7 +5516,7 @@
       <c r="J94" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K94" s="13" t="s">
+      <c r="K94" s="14" t="s">
         <v>89</v>
       </c>
       <c r="L94" s="0"/>
@@ -5548,7 +5561,7 @@
       <c r="J95" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K95" s="13" t="s">
+      <c r="K95" s="14" t="s">
         <v>90</v>
       </c>
       <c r="L95" s="0"/>
@@ -5593,7 +5606,7 @@
       <c r="J96" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K96" s="13" t="s">
+      <c r="K96" s="14" t="s">
         <v>89</v>
       </c>
       <c r="L96" s="0"/>
@@ -5638,7 +5651,7 @@
       <c r="J97" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K97" s="13" t="s">
+      <c r="K97" s="14" t="s">
         <v>90</v>
       </c>
       <c r="L97" s="0"/>
@@ -5683,7 +5696,7 @@
       <c r="J98" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K98" s="13" t="s">
+      <c r="K98" s="14" t="s">
         <v>87</v>
       </c>
       <c r="L98" s="0"/>
@@ -5725,10 +5738,10 @@
       <c r="I99" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J99" s="14" t="s">
+      <c r="J99" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="K99" s="15" t="s">
+      <c r="K99" s="16" t="s">
         <v>94</v>
       </c>
       <c r="L99" s="0"/>
@@ -5772,7 +5785,7 @@
       <c r="J100" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K100" s="13" t="s">
+      <c r="K100" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L100" s="0"/>
@@ -5816,7 +5829,7 @@
       <c r="J101" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K101" s="13" t="s">
+      <c r="K101" s="14" t="s">
         <v>98</v>
       </c>
       <c r="L101" s="0"/>
@@ -5856,10 +5869,10 @@
       <c r="I102" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J102" s="14" t="s">
+      <c r="J102" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="K102" s="15" t="s">
+      <c r="K102" s="16" t="s">
         <v>94</v>
       </c>
       <c r="L102" s="0"/>
@@ -5904,7 +5917,7 @@
       <c r="J103" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K103" s="13" t="s">
+      <c r="K103" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L103" s="0"/>
@@ -5946,10 +5959,10 @@
       <c r="I104" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J104" s="14" t="s">
+      <c r="J104" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="K104" s="15" t="s">
+      <c r="K104" s="16" t="s">
         <v>94</v>
       </c>
       <c r="L104" s="0"/>
@@ -5994,7 +6007,7 @@
       <c r="J105" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K105" s="13" t="s">
+      <c r="K105" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L105" s="0"/>
@@ -6036,10 +6049,10 @@
       <c r="I106" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J106" s="14" t="s">
+      <c r="J106" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="K106" s="15" t="s">
+      <c r="K106" s="16" t="s">
         <v>94</v>
       </c>
       <c r="L106" s="0"/>
@@ -6084,7 +6097,7 @@
       <c r="J107" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K107" s="13" t="s">
+      <c r="K107" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L107" s="0"/>
@@ -6126,10 +6139,10 @@
       <c r="I108" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J108" s="14" t="s">
+      <c r="J108" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="K108" s="15" t="s">
+      <c r="K108" s="16" t="s">
         <v>94</v>
       </c>
       <c r="L108" s="0"/>
@@ -6174,7 +6187,7 @@
       <c r="J109" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K109" s="13" t="s">
+      <c r="K109" s="14" t="s">
         <v>95</v>
       </c>
       <c r="L109" s="0"/>
@@ -6219,7 +6232,7 @@
       <c r="J110" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K110" s="13" t="s">
+      <c r="K110" s="14" t="s">
         <v>102</v>
       </c>
       <c r="L110" s="0"/>
@@ -6263,7 +6276,7 @@
       <c r="J111" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K111" s="13" t="s">
+      <c r="K111" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L111" s="0"/>
@@ -6307,7 +6320,7 @@
       <c r="J112" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K112" s="13" t="s">
+      <c r="K112" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L112" s="0"/>
@@ -6352,7 +6365,7 @@
       <c r="J113" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K113" s="13" t="s">
+      <c r="K113" s="14" t="s">
         <v>102</v>
       </c>
       <c r="L113" s="0"/>
@@ -6397,7 +6410,7 @@
       <c r="J114" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K114" s="13" t="s">
+      <c r="K114" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L114" s="0"/>
@@ -6442,7 +6455,7 @@
       <c r="J115" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K115" s="13" t="s">
+      <c r="K115" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L115" s="0"/>
@@ -6487,7 +6500,7 @@
       <c r="J116" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K116" s="13" t="s">
+      <c r="K116" s="14" t="s">
         <v>102</v>
       </c>
       <c r="L116" s="0"/>
@@ -6532,7 +6545,7 @@
       <c r="J117" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K117" s="13" t="s">
+      <c r="K117" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L117" s="0"/>
@@ -6577,7 +6590,7 @@
       <c r="J118" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K118" s="13" t="s">
+      <c r="K118" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L118" s="0"/>
@@ -6622,7 +6635,7 @@
       <c r="J119" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K119" s="13" t="s">
+      <c r="K119" s="14" t="s">
         <v>102</v>
       </c>
       <c r="L119" s="0"/>
@@ -6667,7 +6680,7 @@
       <c r="J120" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K120" s="13" t="s">
+      <c r="K120" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L120" s="0"/>
@@ -6712,7 +6725,7 @@
       <c r="J121" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K121" s="13" t="s">
+      <c r="K121" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L121" s="0"/>
@@ -6757,7 +6770,7 @@
       <c r="J122" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K122" s="13" t="s">
+      <c r="K122" s="14" t="s">
         <v>102</v>
       </c>
       <c r="L122" s="0"/>
@@ -6802,7 +6815,7 @@
       <c r="J123" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K123" s="13" t="s">
+      <c r="K123" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L123" s="0"/>
@@ -6847,7 +6860,7 @@
       <c r="J124" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K124" s="13" t="s">
+      <c r="K124" s="14" t="s">
         <v>104</v>
       </c>
       <c r="L124" s="0"/>
@@ -6892,7 +6905,7 @@
       <c r="J125" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K125" s="13" t="s">
+      <c r="K125" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L125" s="0"/>
@@ -6936,7 +6949,7 @@
       <c r="J126" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K126" s="13" t="s">
+      <c r="K126" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L126" s="0"/>
@@ -6981,7 +6994,7 @@
       <c r="J127" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K127" s="13" t="s">
+      <c r="K127" s="14" t="s">
         <v>111</v>
       </c>
       <c r="L127" s="0"/>
@@ -7025,7 +7038,7 @@
       <c r="J128" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K128" s="13" t="s">
+      <c r="K128" s="14" t="s">
         <v>113</v>
       </c>
       <c r="L128" s="0"/>
@@ -7069,7 +7082,7 @@
       <c r="J129" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K129" s="13" t="s">
+      <c r="K129" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L129" s="0"/>
@@ -7114,7 +7127,7 @@
       <c r="J130" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K130" s="13" t="s">
+      <c r="K130" s="14" t="s">
         <v>113</v>
       </c>
       <c r="L130" s="0"/>
@@ -7159,7 +7172,7 @@
       <c r="J131" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K131" s="13" t="s">
+      <c r="K131" s="14" t="s">
         <v>111</v>
       </c>
       <c r="L131" s="0"/>
@@ -7204,7 +7217,7 @@
       <c r="J132" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K132" s="13" t="s">
+      <c r="K132" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L132" s="0"/>
@@ -7249,7 +7262,7 @@
       <c r="J133" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K133" s="13" t="s">
+      <c r="K133" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L133" s="0"/>
@@ -7294,7 +7307,7 @@
       <c r="J134" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K134" s="13" t="s">
+      <c r="K134" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L134" s="0"/>
@@ -7339,7 +7352,7 @@
       <c r="J135" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K135" s="13" t="s">
+      <c r="K135" s="14" t="s">
         <v>111</v>
       </c>
       <c r="L135" s="0"/>
@@ -7384,7 +7397,7 @@
       <c r="J136" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K136" s="13" t="s">
+      <c r="K136" s="14" t="s">
         <v>113</v>
       </c>
       <c r="L136" s="0"/>
@@ -7429,7 +7442,7 @@
       <c r="J137" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K137" s="13" t="s">
+      <c r="K137" s="14" t="s">
         <v>111</v>
       </c>
       <c r="L137" s="0"/>
@@ -7474,7 +7487,7 @@
       <c r="J138" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K138" s="13" t="s">
+      <c r="K138" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L138" s="0"/>
@@ -7519,7 +7532,7 @@
       <c r="J139" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K139" s="13" t="s">
+      <c r="K139" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L139" s="0"/>
@@ -7564,7 +7577,7 @@
       <c r="J140" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K140" s="13" t="s">
+      <c r="K140" s="14" t="s">
         <v>113</v>
       </c>
       <c r="L140" s="0"/>
@@ -7609,7 +7622,7 @@
       <c r="J141" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K141" s="13" t="s">
+      <c r="K141" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L141" s="0"/>
@@ -7654,7 +7667,7 @@
       <c r="J142" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K142" s="13" t="s">
+      <c r="K142" s="14" t="s">
         <v>108</v>
       </c>
       <c r="L142" s="0"/>
@@ -7699,7 +7712,7 @@
       <c r="J143" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K143" s="13" t="s">
+      <c r="K143" s="14" t="s">
         <v>111</v>
       </c>
       <c r="L143" s="0"/>
@@ -7744,7 +7757,7 @@
       <c r="J144" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K144" s="13" t="s">
+      <c r="K144" s="14" t="s">
         <v>113</v>
       </c>
       <c r="L144" s="0"/>
@@ -8039,7 +8052,7 @@
       <c r="J150" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K150" s="14" t="s">
+      <c r="K150" s="15" t="s">
         <v>94</v>
       </c>
       <c r="L150" s="0"/>
@@ -8935,7 +8948,7 @@
       <c r="K167" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L167" s="16" t="s">
+      <c r="L167" s="17" t="s">
         <v>146</v>
       </c>
       <c r="M167" s="2" t="n">
@@ -8949,7 +8962,7 @@
       <c r="O167" s="8" t="n">
         <v>3312</v>
       </c>
-      <c r="P167" s="17" t="n">
+      <c r="P167" s="18" t="n">
         <v>4012</v>
       </c>
       <c r="Q167" s="0" t="n">
@@ -11772,86 +11785,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="16" min="14" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+    <row r="1" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="19" t="s">
         <v>186</v>
       </c>
     </row>
@@ -11887,10 +11900,10 @@
         <f aca="false">mapping!M110</f>
         <v>1001</v>
       </c>
-      <c r="N2" s="17" t="n">
+      <c r="N2" s="18" t="n">
         <v>2300</v>
       </c>
-      <c r="O2" s="17" t="n">
+      <c r="O2" s="18" t="n">
         <v>3400</v>
       </c>
     </row>
@@ -11926,10 +11939,10 @@
         <f aca="false">mapping!M125</f>
         <v>1005</v>
       </c>
-      <c r="N3" s="17" t="n">
+      <c r="N3" s="18" t="n">
         <v>2301</v>
       </c>
-      <c r="O3" s="17" t="n">
+      <c r="O3" s="18" t="n">
         <v>3401</v>
       </c>
     </row>
@@ -11965,10 +11978,10 @@
         <f aca="false">M3</f>
         <v>1005</v>
       </c>
-      <c r="N4" s="17" t="n">
+      <c r="N4" s="18" t="n">
         <v>2302</v>
       </c>
-      <c r="O4" s="17" t="n">
+      <c r="O4" s="18" t="n">
         <v>3402</v>
       </c>
     </row>
@@ -12004,10 +12017,10 @@
         <f aca="false">mapping!M87</f>
         <v>1004</v>
       </c>
-      <c r="N5" s="17" t="n">
+      <c r="N5" s="18" t="n">
         <v>2303</v>
       </c>
-      <c r="O5" s="17" t="n">
+      <c r="O5" s="18" t="n">
         <v>3403</v>
       </c>
     </row>
@@ -12043,10 +12056,10 @@
         <f aca="false">M5</f>
         <v>1004</v>
       </c>
-      <c r="N6" s="17" t="n">
+      <c r="N6" s="18" t="n">
         <v>2304</v>
       </c>
-      <c r="O6" s="17" t="n">
+      <c r="O6" s="18" t="n">
         <v>3404</v>
       </c>
       <c r="Q6" s="0" t="n">
@@ -12091,10 +12104,10 @@
         <f aca="false">mapping!M101</f>
         <v>1010</v>
       </c>
-      <c r="N7" s="17" t="n">
+      <c r="N7" s="18" t="n">
         <v>2305</v>
       </c>
-      <c r="O7" s="17" t="n">
+      <c r="O7" s="18" t="n">
         <v>3405</v>
       </c>
     </row>
@@ -12130,10 +12143,10 @@
         <f aca="false">mapping!M72</f>
         <v>1007</v>
       </c>
-      <c r="N8" s="17" t="n">
+      <c r="N8" s="18" t="n">
         <v>2306</v>
       </c>
-      <c r="O8" s="17" t="n">
+      <c r="O8" s="18" t="n">
         <v>3406</v>
       </c>
     </row>
@@ -12169,10 +12182,10 @@
         <f aca="false">M8</f>
         <v>1007</v>
       </c>
-      <c r="N9" s="17" t="n">
+      <c r="N9" s="18" t="n">
         <v>2307</v>
       </c>
-      <c r="O9" s="17" t="n">
+      <c r="O9" s="18" t="n">
         <v>3407</v>
       </c>
     </row>
@@ -12230,7 +12243,7 @@
         <f aca="false">mapping!O167</f>
         <v>3312</v>
       </c>
-      <c r="P10" s="17" t="n">
+      <c r="P10" s="18" t="n">
         <v>4050</v>
       </c>
       <c r="Q10" s="0" t="n">
@@ -12282,7 +12295,7 @@
         <f aca="false">mapping!N25</f>
         <v>2012</v>
       </c>
-      <c r="O11" s="17" t="n">
+      <c r="O11" s="18" t="n">
         <v>3408</v>
       </c>
       <c r="Q11" s="0" t="n">
@@ -12321,10 +12334,10 @@
         <f aca="false">mapping!M63</f>
         <v>1008</v>
       </c>
-      <c r="N12" s="17" t="n">
+      <c r="N12" s="18" t="n">
         <v>2308</v>
       </c>
-      <c r="O12" s="17" t="n">
+      <c r="O12" s="18" t="n">
         <v>3409</v>
       </c>
     </row>
@@ -12360,39 +12373,39 @@
         <f aca="false">M12</f>
         <v>1008</v>
       </c>
-      <c r="N13" s="17" t="n">
+      <c r="N13" s="18" t="n">
         <v>2309</v>
       </c>
-      <c r="O13" s="17" t="n">
+      <c r="O13" s="18" t="n">
         <v>3410</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="17" t="s">
         <v>223</v>
       </c>
       <c r="M14" s="0" t="n">
@@ -12406,31 +12419,31 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="17" t="s">
         <v>218</v>
       </c>
       <c r="M15" s="0" t="n">

</xml_diff>